<commit_message>
Completed mapping and final schema changes for the VT Citation.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/ECF_Court_Filing_Service/artifacts/service_model/information_model/ECF_Court_Filing_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/ECF_Court_Filing_Service/artifacts/service_model/information_model/ECF_Court_Filing_IEPD/documentation/impl-artifacts/vermont/Incident_Ticket_Mapping.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="5260" yWindow="2780" windowWidth="29840" windowHeight="15880"/>
   </bookViews>
   <sheets>
-    <sheet name="Citation" sheetId="1" r:id="rId1"/>
+    <sheet name="eCitation" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="361">
   <si>
     <t>Description</t>
   </si>
@@ -498,9 +498,6 @@
     <t>City Relief Act Other Text</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Commerical Vehicle Indicator</t>
   </si>
   <si>
@@ -609,10 +606,6 @@
     <t>Posteds peed unit of measure</t>
   </si>
   <si>
-    <t>eCitation Element
-(Elements in RED are OJB extensions to the base Incident)</t>
-  </si>
-  <si>
     <t>Vermont eCitation Element</t>
   </si>
   <si>
@@ -776,9 +769,6 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Offense[ndexia:ActivityAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense']/@s:id]/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>We need to add a MTOM attachment that contains a PDF representation of the citation</t>
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CitationServedDate/nc:Date</t>
@@ -893,6 +883,242 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Highlighted elements are not in the ECF subset
+ECF extension elements are in red.</t>
+  </si>
+  <si>
+    <t>eCitation Element
+(Elements in RED are OJB extensions to ECF)</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationWaiverAmount</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationServedIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationMailedIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/ojb-cit-ext:DriverLicenseCDLIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleCMVIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/ojb-cit-ext:VehicleAugmentation/ojb-cit-ext:VehicleHazardousMaterialIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]//ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayPositionText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/ecf-cit:PersonBloodAlcoholNumber</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:DrivingAccidentFatalityIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:IncidentAugmentation/j:IncidentTrafficAccidentInvolvedIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:SeatBeltViolationIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseViolatedStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:CFRStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteOffenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:RelatedCriminalChargeIndicator</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:DrivingOffensePoints</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMinimum</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMaximum</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsHomeIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsWorkIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1341,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="530">
+  <cellStyleXfs count="728">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1646,8 +1872,206 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1700,20 +2124,29 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="530">
+  <cellStyles count="728">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1987,6 +2420,105 @@
     <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2239,6 +2771,105 @@
     <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2542,11 +3173,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2555,21 +3186,21 @@
     <col min="2" max="2" width="39.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.83203125" style="10" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="100.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="48.1640625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1" ht="42">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="28">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>284</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>124</v>
@@ -2578,1378 +3209,1586 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19" customHeight="1">
+      <c r="A2" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="13"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="70">
-      <c r="A4" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D4" s="2">
+    <row r="3" spans="1:6" ht="70">
+      <c r="A3" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="2">
         <v>82734800</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>215</v>
+      <c r="E3" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A4" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7">
+        <v>42304</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A5" s="6" t="s">
-        <v>199</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="7">
-        <v>42304</v>
+        <v>48</v>
+      </c>
+      <c r="D5" s="8">
+        <v>105</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>252</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="8">
-        <v>105</v>
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="F6" s="8"/>
+        <v>251</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A7" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="70">
+      <c r="A9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="70">
+      <c r="A11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="70">
+      <c r="A13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="70">
+      <c r="A14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="70">
+      <c r="A15" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="112">
+      <c r="A16" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="112">
+      <c r="A17" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="140">
+      <c r="A18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="84">
+      <c r="A20" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="70">
-      <c r="A10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="70">
-      <c r="A12" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="70">
-      <c r="A14" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="70">
-      <c r="A15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2">
+        <v>41444812</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="70">
-      <c r="A16" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="15" t="s">
+      <c r="F20" s="21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="84">
+      <c r="A21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="112">
-      <c r="A17" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="112">
-      <c r="A18" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="140">
-      <c r="A19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A20" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="84">
-      <c r="A21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2">
-        <v>41444812</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="84">
+      <c r="F21" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="140">
       <c r="A22" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="140">
-      <c r="A23" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2">
-        <v>12345678</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>260</v>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3">
+        <v>8023631111</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A24" s="6" t="s">
-        <v>16</v>
+      <c r="A24" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="3">
-        <v>8023631111</v>
+        <v>8023631112</v>
       </c>
       <c r="E24" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="7">
+        <v>24014</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" ht="56">
+      <c r="A27" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="3">
-        <v>8023631112</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A26" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="7">
-        <v>24014</v>
-      </c>
-      <c r="E26" s="15" t="s">
+      <c r="F27" s="21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A27" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="15" t="s">
+      <c r="F28" s="21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A29" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1">
-      <c r="A28" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A29" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="3">
         <v>135</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A30" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="F30" s="21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E31" s="15" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A31" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="3">
-        <v>135</v>
-      </c>
-      <c r="E31" s="15" t="s">
+      <c r="F31" s="21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A32" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A32" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>226</v>
+      <c r="F32" s="21" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A34" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A36" s="19" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A35" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="B35" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A36" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="B36" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="E36" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A37" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A38" s="19" t="s">
-        <v>98</v>
+      <c r="F37" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A38" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>174</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>125</v>
+        <v>24</v>
+      </c>
+      <c r="D38" s="3">
+        <v>2015</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>211</v>
+        <v>206</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A39" s="19" t="s">
-        <v>99</v>
+      <c r="A39" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>175</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="3">
-        <v>2015</v>
+        <v>25</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>208</v>
+        <v>210</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A40" s="19" t="s">
-        <v>100</v>
+      <c r="A40" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>176</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A41" s="19" t="s">
-        <v>101</v>
+      <c r="A41" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A42" s="19" t="s">
-        <v>102</v>
+        <v>212</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A42" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>178</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>141</v>
+        <v>39</v>
+      </c>
+      <c r="D42" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>214</v>
+        <v>258</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A43" s="21" t="s">
-        <v>160</v>
+      <c r="A43" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>179</v>
+        <v>76</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A44" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" s="3" customFormat="1" ht="68" customHeight="1">
+      <c r="A45" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A46" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="3" customFormat="1" ht="126">
+      <c r="A47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A48" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A49" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="3">
+        <v>30</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A53" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="3">
         <v>40</v>
       </c>
-      <c r="D44" s="3" t="b">
+      <c r="E54" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A55" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="3" t="b">
         <v>0</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A46" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A47" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" ht="126">
-      <c r="A48" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A49" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A50" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A51" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A52" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A53" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="3">
-        <v>30</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A54" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A55" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D55" s="3">
-        <v>40</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A56" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>234</v>
       </c>
+      <c r="F56" s="21" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A57" s="19" t="s">
-        <v>111</v>
+      <c r="A57" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D57" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A58" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D58" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E58" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="70">
+      <c r="A59" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A59" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>238</v>
+      <c r="F59" s="21" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="70">
-      <c r="A60" s="20" t="s">
-        <v>118</v>
+      <c r="A60" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="70">
-      <c r="A61" s="20" t="s">
-        <v>119</v>
+      <c r="A61" s="18" t="s">
+        <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D61" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="E61" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="70">
+      <c r="A62" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="70">
-      <c r="A62" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" s="10" t="s">
+      <c r="F62" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A64" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A65" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A66" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="70">
-      <c r="A63" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="5"/>
-    </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A65" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A66" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>244</v>
+      <c r="F66" s="3" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A67" s="6" t="s">
-        <v>166</v>
+      <c r="A67" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>243</v>
       </c>
+      <c r="F67" s="3" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A68" s="19" t="s">
-        <v>115</v>
+      <c r="A68" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>79</v>
+        <v>192</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>150</v>
+        <v>57</v>
+      </c>
+      <c r="D68" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A69" s="6" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D69" s="3" t="b">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="D69" s="3">
+        <v>2</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F69" s="6"/>
+        <v>244</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="70" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A70" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D70" s="3">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="D70" s="8">
+        <v>47</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A71" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D71" s="8">
-        <v>47</v>
+        <v>1197</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="F71" s="8"/>
-    </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A72" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D72" s="8">
-        <v>1197</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="F72" s="8"/>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A74" s="6" t="s">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A73" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="B73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A74" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="B74" s="3" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>151</v>
+        <v>52</v>
+      </c>
+      <c r="D74" s="3">
+        <v>12345</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A75" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>117</v>
+        <v>275</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1">
+      <c r="A75" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D75" s="3">
-        <v>12345</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="3" customFormat="1">
+        <v>54</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A76" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>54</v>
+        <v>143</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E76" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" ht="70">
+      <c r="A79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="70">
+      <c r="A80" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="112">
+      <c r="A81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="112">
+      <c r="A82" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="126">
+      <c r="A83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="112">
+      <c r="A84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:6" ht="84">
+      <c r="A86" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="119" customHeight="1">
+      <c r="A87" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A77" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A78" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80" spans="1:6" ht="70">
-      <c r="A80" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" ht="70">
-      <c r="A81" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="112">
-      <c r="A82" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="1:6" ht="112">
-      <c r="A83" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="F83" s="3"/>
-    </row>
-    <row r="84" spans="1:6" ht="126">
-      <c r="A84" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E84" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" ht="112">
-      <c r="A85" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87" spans="1:6" ht="84">
-      <c r="A87" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="119" customHeight="1">
-      <c r="A88" s="2" t="s">
-        <v>252</v>
-      </c>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A87:E87"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>

</xml_diff>